<commit_message>
MAJ mapping suite review de NRISS 39b045f35aead0577830ffad59c0bbbf16e0bb22
</commit_message>
<xml_diff>
--- a/mappingCorps/ig/FRActLMCDAFHIR.xlsx
+++ b/mappingCorps/ig/FRActLMCDAFHIR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
   <si>
     <t>Property</t>
   </si>
@@ -37,15 +37,12 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
     <t>Mapping Métier/CDA/FHIR : "Acte"</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Mapping FRLMActe → FRCDAActe → FRProcedureActDocument</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -58,7 +55,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-05T15:47:03+00:00</t>
+    <t>2026-01-07T15:20:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -196,7 +193,7 @@
     <t>FRLMActe.circonstances</t>
   </si>
   <si>
-    <t>FRCDAActe.entryRelationship.frReferenceInterne</t>
+    <t>FRCDAActe.entryRelationship:frReferenceInterne</t>
   </si>
   <si>
     <t>FRLMActe.reason</t>
@@ -208,12 +205,15 @@
     <t>FRLMActe.difficulte</t>
   </si>
   <si>
-    <t>FRCDAActe.entryRelationship.frSimpleObservation</t>
+    <t>FRCDAActe.entryRelationship:frSimpleObservationDifficulte</t>
   </si>
   <si>
     <t>FRLMActe.scores</t>
   </si>
   <si>
+    <t>FRCDAActe.entryRelationship:frSimpleObservationScores</t>
+  </si>
+  <si>
     <t>https://interop.esante.gouv.fr/ig/document/core/StructureDefinition/fr-procedure-act-document</t>
   </si>
   <si>
@@ -235,34 +235,46 @@
     <t>FRProcedureActDocument.status</t>
   </si>
   <si>
+    <t>FRCDAActe.entryRelationship:frReferenceInterneDM</t>
+  </si>
+  <si>
     <t>FRProcedureActDocument.usedReference</t>
   </si>
   <si>
+    <t>FRCDAActe.entryRelationship:frSimpleObservationObservationsLiees</t>
+  </si>
+  <si>
     <t>FRProcedureActDocument.partOf</t>
   </si>
   <si>
-    <t>FRProcedureActDocument.performer.actor.extension.Intervenant</t>
-  </si>
-  <si>
-    <t>FRProcedureActDocument.performer.actor.extension.Informateur</t>
-  </si>
-  <si>
-    <t>FRProcedureActDocument.performer.actor.extension.Participant</t>
+    <t>FRProcedureActDocument.performer.actor.extension:Intervenant</t>
+  </si>
+  <si>
+    <t>FRProcedureActDocument.performer.actor.extension:Informateur</t>
+  </si>
+  <si>
+    <t>FRProcedureActDocument.performer.actor.extension:Participant</t>
+  </si>
+  <si>
+    <t>FRCDAActe.entryRelationship:frReferenceInterneMotifActe</t>
   </si>
   <si>
     <t>FRProcedureActDocument.reasonReference</t>
   </si>
   <si>
+    <t>FRCDAActe.entryRelationship:frReferenceInterneRencontreAssociee</t>
+  </si>
+  <si>
     <t>FRProcedureActDocument.encounter</t>
   </si>
   <si>
-    <t>FRProcedureActDocument.recorder.extension.author</t>
+    <t>FRProcedureActDocument.recorder.extension:author</t>
   </si>
   <si>
     <t>priorityCode</t>
   </si>
   <si>
-    <t>FRProcedureActDocument.extension.priority</t>
+    <t>FRProcedureActDocument.extension:priority</t>
   </si>
   <si>
     <t>FRProcedureActDocument.bodySite.TargetSiteCode</t>
@@ -440,81 +452,79 @@
       <c r="A4" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>7</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="2">
         <v>8</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="2">
         <v>10</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>13</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>15</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>17</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>19</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>21</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -533,269 +543,269 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>25</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="C1" t="s" s="1">
         <v>26</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="D1" t="s" s="1">
         <v>27</v>
       </c>
-      <c r="D1" t="s" s="1">
-        <v>28</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="C2" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>31</v>
-      </c>
       <c r="E2" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
         <v>33</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>34</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E20" s="2"/>
     </row>
@@ -814,45 +824,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>25</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="C1" t="s" s="1">
         <v>26</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="D1" t="s" s="1">
         <v>27</v>
       </c>
-      <c r="D1" t="s" s="1">
-        <v>28</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s" s="2">
         <v>66</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>67</v>
@@ -861,11 +871,11 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s" s="2">
         <v>68</v>
@@ -874,11 +884,11 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
         <v>69</v>
@@ -887,11 +897,11 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
         <v>70</v>
@@ -900,11 +910,11 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s" s="2">
         <v>71</v>
@@ -913,11 +923,11 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
         <v>72</v>
@@ -926,144 +936,144 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2"/>
     </row>

</xml_diff>

<commit_message>
MAJ mapping suite review de NRISS b4db2346a4970037c5b65a1e627f3152e9c8781a
</commit_message>
<xml_diff>
--- a/mappingCorps/ig/FRActLMCDAFHIR.xlsx
+++ b/mappingCorps/ig/FRActLMCDAFHIR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
   <si>
     <t>Property</t>
   </si>
@@ -55,7 +55,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-07T15:20:53+00:00</t>
+    <t>2026-01-07T21:00:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -193,15 +193,21 @@
     <t>FRLMActe.circonstances</t>
   </si>
   <si>
-    <t>FRCDAActe.entryRelationship:frReferenceInterne</t>
+    <t>FRCDAActe.entryRelationship:frReferenceInterneCirconstances</t>
   </si>
   <si>
     <t>FRLMActe.reason</t>
   </si>
   <si>
+    <t>FRCDAActe.entryRelationship:frReferenceInterneMotifActe</t>
+  </si>
+  <si>
     <t>FRLMActe.dispositifMedical</t>
   </si>
   <si>
+    <t>FRCDAActe.entryRelationship:frReferenceInterneDM</t>
+  </si>
+  <si>
     <t>FRLMActe.difficulte</t>
   </si>
   <si>
@@ -235,15 +241,9 @@
     <t>FRProcedureActDocument.status</t>
   </si>
   <si>
-    <t>FRCDAActe.entryRelationship:frReferenceInterneDM</t>
-  </si>
-  <si>
     <t>FRProcedureActDocument.usedReference</t>
   </si>
   <si>
-    <t>FRCDAActe.entryRelationship:frSimpleObservationObservationsLiees</t>
-  </si>
-  <si>
     <t>FRProcedureActDocument.partOf</t>
   </si>
   <si>
@@ -256,16 +256,13 @@
     <t>FRProcedureActDocument.performer.actor.extension:Participant</t>
   </si>
   <si>
-    <t>FRCDAActe.entryRelationship:frReferenceInterneMotifActe</t>
-  </si>
-  <si>
     <t>FRProcedureActDocument.reasonReference</t>
   </si>
   <si>
-    <t>FRCDAActe.entryRelationship:frReferenceInterneRencontreAssociee</t>
-  </si>
-  <si>
     <t>FRProcedureActDocument.encounter</t>
+  </si>
+  <si>
+    <t>FRProcedureActDocument.extension:difficulte</t>
   </si>
   <si>
     <t>FRProcedureActDocument.recorder.extension:author</t>
@@ -766,46 +763,46 @@
         <v>32</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E20" s="2"/>
     </row>
@@ -816,7 +813,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -850,7 +847,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>29</v>
@@ -865,7 +862,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -878,7 +875,7 @@
         <v>32</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -891,7 +888,7 @@
         <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -904,7 +901,7 @@
         <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -917,7 +914,7 @@
         <v>32</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -930,26 +927,26 @@
         <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -1001,81 +998,94 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="E20" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>